<commit_message>
animus lvl fix & rename cora force to animus npc
</commit_message>
<xml_diff>
--- a/gu_in/Character.edf/Action.xlsx
+++ b/gu_in/Character.edf/Action.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr filterPrivacy="true"/>
+  <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CB2EC4-63C2-4E10-8204-3689A17990FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="285" windowWidth="24930" windowHeight="15105"/>
+    <workbookView xWindow="1650" yWindow="285" windowWidth="24930" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cliaction" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="true"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>string[32]</t>
   </si>
@@ -155,20 +155,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -183,15 +178,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -474,20 +467,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="6.7109375" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="16.7109375" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="6.7109375" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="4.7109375" bestFit="true" customWidth="true"/>
+    <col min="1" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -507,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -525,651 +518,651 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2">
-        <v>50</v>
+      <c r="E5" s="1">
+        <v>10</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2">
-        <v>50</v>
+      <c r="E6" s="1">
+        <v>10</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2">
-        <v>50</v>
+      <c r="E7" s="1">
+        <v>10</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2">
-        <v>50</v>
+      <c r="E8" s="1">
+        <v>10</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2">
-        <v>50</v>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>10</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2">
-        <v>50</v>
+      <c r="E10" s="1">
+        <v>10</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="2">
-        <v>50</v>
+      <c r="E11" s="1">
+        <v>10</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="2">
-        <v>50</v>
+      <c r="E12" s="1">
+        <v>10</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
         <v>11</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2">
-        <v>50</v>
+      <c r="E13" s="1">
+        <v>10</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="2">
-        <v>50</v>
+      <c r="E14" s="1">
+        <v>10</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="2">
-        <v>50</v>
+      <c r="E15" s="1">
+        <v>10</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="2">
-        <v>50</v>
+      <c r="E16" s="1">
+        <v>10</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="2">
-        <v>50</v>
+      <c r="E17" s="1">
+        <v>10</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
         <v>15</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="2">
-        <v>50</v>
+      <c r="E18" s="1">
+        <v>10</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="2">
-        <v>50</v>
+      <c r="E19" s="1">
+        <v>10</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>21</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="2">
-        <v>50</v>
+      <c r="E20" s="1">
+        <v>0</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="2">
-        <v>50</v>
+      <c r="E21" s="1">
+        <v>0</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>26</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="2">
-        <v>50</v>
+      <c r="E22" s="1">
+        <v>1</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>0</v>
-      </c>
-      <c r="B23" s="2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>27</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="2">
-        <v>50</v>
+      <c r="E23" s="1">
+        <v>1</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>32</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="2">
-        <v>50</v>
+      <c r="E24" s="1">
+        <v>7</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>0</v>
-      </c>
-      <c r="B25" s="2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>31</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="2">
-        <v>50</v>
+      <c r="E25" s="1">
+        <v>7</v>
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>0</v>
-      </c>
-      <c r="B26" s="2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>24</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="2">
-        <v>50</v>
+      <c r="E26" s="1">
+        <v>7</v>
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>0</v>
-      </c>
-      <c r="B27" s="2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>30</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="2">
-        <v>50</v>
+      <c r="E27" s="1">
+        <v>2</v>
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>0</v>
-      </c>
-      <c r="B28" s="2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>33</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="2">
-        <v>50</v>
+      <c r="E28" s="1">
+        <v>2</v>
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>0</v>
-      </c>
-      <c r="B29" s="2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>25</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="2">
-        <v>50</v>
+      <c r="E29" s="1">
+        <v>3</v>
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>0</v>
-      </c>
-      <c r="B30" s="2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>36</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="2">
-        <v>50</v>
+      <c r="E30" s="1">
+        <v>3</v>
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
         <v>28</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>34</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="2">
-        <v>50</v>
+      <c r="E31" s="1">
+        <v>8</v>
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
         <v>29</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>37</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="2">
-        <v>50</v>
+      <c r="E32" s="1">
+        <v>8</v>
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>0</v>
-      </c>
-      <c r="B33" s="2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1">
         <v>30</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>29</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="2">
-        <v>50</v>
+      <c r="E33" s="1">
+        <v>8</v>
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>0</v>
-      </c>
-      <c r="B34" s="2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1">
         <v>31</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>23</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="2">
-        <v>50</v>
+      <c r="E34" s="1">
+        <v>4</v>
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>0</v>
-      </c>
-      <c r="B35" s="2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
         <v>32</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>19</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="2">
-        <v>50</v>
+      <c r="E35" s="1">
+        <v>4</v>
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>0</v>
-      </c>
-      <c r="B36" s="2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1">
         <v>33</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>38</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="2">
-        <v>50</v>
+      <c r="E36" s="1">
+        <v>4</v>
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>0</v>
-      </c>
-      <c r="B37" s="2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1">
         <v>34</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>35</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="2">
-        <v>50</v>
+      <c r="E37" s="1">
+        <v>4</v>
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>0</v>
-      </c>
-      <c r="B38" s="2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1">
         <v>35</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>22</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="2">
-        <v>50</v>
+      <c r="E38" s="1">
+        <v>4</v>
       </c>
       <c r="F38" s="1"/>
     </row>

</xml_diff>